<commit_message>
Add the 1st/2nd/3rd modified codes:Davy
</commit_message>
<xml_diff>
--- a/Doc/Analysis.xlsx
+++ b/Doc/Analysis.xlsx
@@ -4,13 +4,15 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26819"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14720" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14580" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="工作表1" sheetId="1" r:id="rId1"/>
+    <sheet name="NA Var Stat" sheetId="1" r:id="rId1"/>
+    <sheet name="工作表1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="stat_na" localSheetId="0">工作表1!$B$3:$F$8</definedName>
+    <definedName name="bigCategoryStat" localSheetId="1">工作表1!$B$3:$E$8</definedName>
+    <definedName name="stat_na" localSheetId="0">'NA Var Stat'!$B$3:$F$8</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -23,7 +25,17 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="stat_na.csv" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="1" name="bigCategoryStat.csv" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" codePage="10008" sourceFile="studio:Kesci-Mojing:Mojing:Doc:bigCategoryStat.csv" space="1" consecutive="1">
+      <textFields count="4">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="2" name="stat_na.csv" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" codePage="10008" sourceFile="studio:Kesci-Mojing:Mojing:Doc:stat_na.csv" space="1" comma="1" consecutive="1">
       <textFields count="4">
         <textField/>
@@ -37,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>id</t>
   </si>
@@ -68,6 +80,39 @@
   </si>
   <si>
     <t>Variables</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Stat for NA Vaviables</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>colNames</t>
+  </si>
+  <si>
+    <t>idx</t>
+  </si>
+  <si>
+    <t>UserInfo_3</t>
+  </si>
+  <si>
+    <t>WeblogInfo_4</t>
+  </si>
+  <si>
+    <t>UserInfo_14</t>
+  </si>
+  <si>
+    <t>Education_Info1</t>
+  </si>
+  <si>
+    <t>Education_Info5</t>
+  </si>
+  <si>
+    <t>n</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Stat for Big Categories</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -78,7 +123,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -94,16 +139,55 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -111,18 +195,177 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="普通" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -131,7 +374,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="stat_na" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="stat_na" connectionId="2" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="bigCategoryStat" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -456,10 +703,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:F8"/>
+  <dimension ref="B1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -470,8 +717,18 @@
     <col min="6" max="6" width="6.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="2:6" ht="16" thickBot="1"/>
+    <row r="2" spans="2:6">
+      <c r="B2" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="12"/>
+    </row>
     <row r="3" spans="2:6">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -483,96 +740,204 @@
       <c r="E3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="3" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="2:6">
-      <c r="B4" t="s">
+      <c r="B4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="5">
         <v>6</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="5">
         <v>29030</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="5">
         <v>30000</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4" s="6">
         <v>0.96799999999999997</v>
       </c>
     </row>
     <row r="5" spans="2:6">
-      <c r="B5" t="s">
+      <c r="B5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="5">
         <v>8</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="5">
         <v>29030</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="5">
         <v>30000</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F5" s="6">
         <v>0.96799999999999997</v>
       </c>
     </row>
     <row r="6" spans="2:6">
-      <c r="B6" t="s">
+      <c r="B6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="5">
         <v>30</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="5">
         <v>18909</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="5">
         <v>30000</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6" s="6">
         <v>0.63</v>
       </c>
     </row>
     <row r="7" spans="2:6">
-      <c r="B7" t="s">
+      <c r="B7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="5">
         <v>31</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="5">
         <v>18909</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="5">
         <v>30000</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7" s="6">
         <v>0.63</v>
       </c>
     </row>
-    <row r="8" spans="2:6">
-      <c r="B8" t="s">
+    <row r="8" spans="2:6" ht="16" thickBot="1">
+      <c r="B8" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="8">
         <v>32</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="8">
         <v>18909</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="8">
         <v>30000</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F8" s="9">
         <v>0.63</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:F2"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:D8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="16.83203125" customWidth="1"/>
+    <col min="3" max="3" width="6.83203125" customWidth="1"/>
+    <col min="4" max="4" width="6.5" customWidth="1"/>
+    <col min="5" max="5" width="5.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:4" ht="16" thickBot="1"/>
+    <row r="2" spans="2:4">
+      <c r="B2" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="11"/>
+      <c r="D2" s="12"/>
+    </row>
+    <row r="3" spans="2:4">
+      <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4">
+      <c r="B4" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="14">
+        <v>3</v>
+      </c>
+      <c r="D4" s="15">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4">
+      <c r="B5" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="14">
+        <v>5</v>
+      </c>
+      <c r="D5" s="15">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4">
+      <c r="B6" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="14">
+        <v>25</v>
+      </c>
+      <c r="D6" s="15">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4">
+      <c r="B7" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="14">
+        <v>34</v>
+      </c>
+      <c r="D7" s="15">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" ht="16" thickBot="1">
+      <c r="B8" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="17">
+        <v>38</v>
+      </c>
+      <c r="D8" s="18">
+        <v>1963</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:D2"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Update the latest codes:Davy
</commit_message>
<xml_diff>
--- a/Doc/Analysis.xlsx
+++ b/Doc/Analysis.xlsx
@@ -4,14 +4,15 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26819"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14580" tabRatio="500" activeTab="1"/>
+    <workbookView minimized="1" xWindow="25600" yWindow="2440" windowWidth="16000" windowHeight="10580" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="NA Var Stat" sheetId="1" r:id="rId1"/>
-    <sheet name="工作表1" sheetId="2" r:id="rId2"/>
+    <sheet name="Big Cate Stat" sheetId="2" r:id="rId2"/>
+    <sheet name="工作表1" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="bigCategoryStat" localSheetId="1">工作表1!$B$3:$E$8</definedName>
+    <definedName name="bigCategoryStat" localSheetId="1">'Big Cate Stat'!$B$3:$E$8</definedName>
     <definedName name="stat_na" localSheetId="0">'NA Var Stat'!$B$3:$F$8</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
@@ -49,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>id</t>
   </si>
@@ -113,6 +114,34 @@
   </si>
   <si>
     <t>Stat for Big Categories</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>不详</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>电信</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>移动</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>联通</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1+0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1+0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>手机类型</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -318,7 +347,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -335,6 +364,24 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="176" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -344,22 +391,10 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -706,7 +741,7 @@
   <dimension ref="B1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -719,13 +754,13 @@
   <sheetData>
     <row r="1" spans="2:6" ht="16" thickBot="1"/>
     <row r="2" spans="2:6">
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="12"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="18"/>
     </row>
     <row r="3" spans="2:6">
       <c r="B3" s="1" t="s">
@@ -848,7 +883,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
@@ -862,11 +897,11 @@
   <sheetData>
     <row r="1" spans="2:4" ht="16" thickBot="1"/>
     <row r="2" spans="2:4">
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="12"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="18"/>
     </row>
     <row r="3" spans="2:4">
       <c r="B3" s="1" t="s">
@@ -880,57 +915,57 @@
       </c>
     </row>
     <row r="4" spans="2:4">
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="14">
+      <c r="C4" s="11">
         <v>3</v>
       </c>
-      <c r="D4" s="15">
+      <c r="D4" s="12">
         <v>328</v>
       </c>
     </row>
     <row r="5" spans="2:4">
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="14">
+      <c r="C5" s="11">
         <v>5</v>
       </c>
-      <c r="D5" s="15">
+      <c r="D5" s="12">
         <v>331</v>
       </c>
     </row>
     <row r="6" spans="2:4">
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="14">
+      <c r="C6" s="11">
         <v>25</v>
       </c>
-      <c r="D6" s="15">
+      <c r="D6" s="12">
         <v>655</v>
       </c>
     </row>
     <row r="7" spans="2:4">
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="14">
+      <c r="C7" s="11">
         <v>34</v>
       </c>
-      <c r="D7" s="15">
+      <c r="D7" s="12">
         <v>297</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="16" thickBot="1">
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="17">
+      <c r="C8" s="14">
         <v>38</v>
       </c>
-      <c r="D8" s="18">
+      <c r="D8" s="15">
         <v>1963</v>
       </c>
     </row>
@@ -947,4 +982,188 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:H16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="3" spans="2:8">
+      <c r="B3" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="19">
+        <v>1</v>
+      </c>
+      <c r="D3" s="19">
+        <v>0</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="19">
+        <v>1</v>
+      </c>
+      <c r="G3" s="19">
+        <v>0</v>
+      </c>
+      <c r="H3" s="19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8">
+      <c r="B4" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="19">
+        <v>336</v>
+      </c>
+      <c r="D4" s="19">
+        <v>3877</v>
+      </c>
+      <c r="E4" s="19">
+        <f>SUM(C4:D4)</f>
+        <v>4213</v>
+      </c>
+      <c r="F4" s="20">
+        <f t="shared" ref="F4:F7" si="0">C4/$C$8</f>
+        <v>0.15286624203821655</v>
+      </c>
+      <c r="G4" s="20">
+        <f t="shared" ref="G4:G7" si="1">D4/$D$8</f>
+        <v>0.13945039925185237</v>
+      </c>
+      <c r="H4" s="20">
+        <f t="shared" ref="H4:H7" si="2">E4/$E$8</f>
+        <v>0.14043333333333333</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8">
+      <c r="B5" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="19">
+        <v>224</v>
+      </c>
+      <c r="D5" s="19">
+        <v>2981</v>
+      </c>
+      <c r="E5" s="19">
+        <f t="shared" ref="E5:E7" si="3">SUM(C5:D5)</f>
+        <v>3205</v>
+      </c>
+      <c r="F5" s="20">
+        <f t="shared" si="0"/>
+        <v>0.10191082802547771</v>
+      </c>
+      <c r="G5" s="20">
+        <f t="shared" si="1"/>
+        <v>0.10722250197827495</v>
+      </c>
+      <c r="H5" s="20">
+        <f t="shared" si="2"/>
+        <v>0.10683333333333334</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8">
+      <c r="B6" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="19">
+        <v>1233</v>
+      </c>
+      <c r="D6" s="19">
+        <v>16009</v>
+      </c>
+      <c r="E6" s="19">
+        <f t="shared" si="3"/>
+        <v>17242</v>
+      </c>
+      <c r="F6" s="20">
+        <f t="shared" si="0"/>
+        <v>0.56096451319381258</v>
+      </c>
+      <c r="G6" s="20">
+        <f t="shared" si="1"/>
+        <v>0.57582188331774697</v>
+      </c>
+      <c r="H6" s="20">
+        <f t="shared" si="2"/>
+        <v>0.57473333333333332</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8">
+      <c r="B7" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="19">
+        <v>405</v>
+      </c>
+      <c r="D7" s="19">
+        <v>4935</v>
+      </c>
+      <c r="E7" s="19">
+        <f t="shared" si="3"/>
+        <v>5340</v>
+      </c>
+      <c r="F7" s="20">
+        <f t="shared" si="0"/>
+        <v>0.18425841674249319</v>
+      </c>
+      <c r="G7" s="20">
+        <f t="shared" si="1"/>
+        <v>0.17750521545212575</v>
+      </c>
+      <c r="H7" s="20">
+        <f t="shared" si="2"/>
+        <v>0.17799999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8">
+      <c r="C8" s="19">
+        <f>SUM(C4:C7)</f>
+        <v>2198</v>
+      </c>
+      <c r="D8" s="19">
+        <f>SUM(D4:D7)</f>
+        <v>27802</v>
+      </c>
+      <c r="E8" s="19">
+        <f>SUM(E4:E7)</f>
+        <v>30000</v>
+      </c>
+      <c r="F8" s="20">
+        <f>C8/$C$8</f>
+        <v>1</v>
+      </c>
+      <c r="G8" s="20">
+        <f>D8/$D$8</f>
+        <v>1</v>
+      </c>
+      <c r="H8" s="20">
+        <f>E8/$E$8</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8">
+      <c r="F16">
+        <f>13.9/15.3</f>
+        <v>0.90849673202614378</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>